<commit_message>
modify excel user list and rename institution(s) to service(s) in search
</commit_message>
<xml_diff>
--- a/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFullNew.xlsx
+++ b/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFullNew.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5794" uniqueCount="2713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5795" uniqueCount="2713">
   <si>
     <t>A</t>
   </si>
@@ -10717,7 +10717,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10727,10 +10727,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="X1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection activeCell="C89" sqref="C89"/>
-      <selection pane="topRight" activeCell="AB259" sqref="AB259"/>
+      <selection pane="topRight" activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -14468,7 +14468,7 @@
         <v>779</v>
       </c>
       <c r="AB37" s="55" t="s">
-        <v>1950</v>
+        <v>1925</v>
       </c>
       <c r="AC37" s="55" t="s">
         <v>1923</v>
@@ -21868,7 +21868,7 @@
       <c r="BK111" s="62"/>
       <c r="BL111" s="42"/>
     </row>
-    <row r="112" spans="1:64" s="1" customFormat="1" ht="25.5">
+    <row r="112" spans="1:64" s="1" customFormat="1" ht="45">
       <c r="A112" s="10"/>
       <c r="B112" s="3"/>
       <c r="C112" s="37"/>
@@ -21887,7 +21887,9 @@
       <c r="J112" s="40" t="s">
         <v>1070</v>
       </c>
-      <c r="K112" s="14"/>
+      <c r="K112" s="14" t="s">
+        <v>775</v>
+      </c>
       <c r="L112" s="14"/>
       <c r="M112" s="14"/>
       <c r="N112" s="14"/>

</xml_diff>

<commit_message>
modified excel user list
</commit_message>
<xml_diff>
--- a/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFullNew.xlsx
+++ b/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFullNew.xlsx
@@ -8146,9 +8146,6 @@
     <t>Assistant Director, Molecular Hematopathology;Assistant Director, Molecular Hematopathology</t>
   </si>
   <si>
-    <t>Professor of Pathology and Laboratory Medicine;Professor of Pathology and Laboratory Medicine;Professor of Pathology and Laboratory Medicine</t>
-  </si>
-  <si>
     <t>Director, Cytogenetics;Director, Cytogenetics</t>
   </si>
   <si>
@@ -8171,6 +8168,9 @@
   </si>
   <si>
     <t>Genitourinary Pathology;Genitourinary Pathology</t>
+  </si>
+  <si>
+    <t>Professor of Pathology and Laboratory Medicine;Professor of Pathology and Laboratory Medicine</t>
   </si>
 </sst>
 </file>
@@ -10717,7 +10717,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10727,10 +10727,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="H1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="X1" activePane="topRight" state="frozen"/>
       <selection activeCell="C89" sqref="C89"/>
-      <selection pane="topRight" activeCell="I110" sqref="I110"/>
+      <selection pane="topRight" activeCell="Y37" sqref="Y37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -14459,7 +14459,7 @@
         <v>1918</v>
       </c>
       <c r="Y37" s="46" t="s">
-        <v>2704</v>
+        <v>2712</v>
       </c>
       <c r="Z37" s="5" t="s">
         <v>1919</v>
@@ -29544,16 +29544,16 @@
         <v>1667</v>
       </c>
       <c r="I187" s="43" t="s">
-        <v>2705</v>
+        <v>2704</v>
       </c>
       <c r="J187" s="54" t="s">
         <v>1915</v>
       </c>
       <c r="K187" s="5" t="s">
+        <v>2705</v>
+      </c>
+      <c r="L187" s="5" t="s">
         <v>2706</v>
-      </c>
-      <c r="L187" s="5" t="s">
-        <v>2707</v>
       </c>
       <c r="M187" s="5" t="s">
         <v>855</v>
@@ -35946,16 +35946,16 @@
         <v>1868</v>
       </c>
       <c r="J249" s="14" t="s">
+        <v>2707</v>
+      </c>
+      <c r="K249" s="14" t="s">
+        <v>2705</v>
+      </c>
+      <c r="L249" s="14" t="s">
+        <v>2706</v>
+      </c>
+      <c r="M249" s="14" t="s">
         <v>2708</v>
-      </c>
-      <c r="K249" s="14" t="s">
-        <v>2706</v>
-      </c>
-      <c r="L249" s="14" t="s">
-        <v>2707</v>
-      </c>
-      <c r="M249" s="14" t="s">
-        <v>2709</v>
       </c>
       <c r="N249" s="14"/>
       <c r="O249" s="14"/>
@@ -37074,16 +37074,16 @@
         <v>963</v>
       </c>
       <c r="AB259" s="42" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AC259" s="42" t="s">
+        <v>2705</v>
+      </c>
+      <c r="AD259" s="42" t="s">
         <v>2710</v>
       </c>
-      <c r="AC259" s="42" t="s">
-        <v>2706</v>
-      </c>
-      <c r="AD259" s="42" t="s">
+      <c r="AE259" s="42" t="s">
         <v>2711</v>
-      </c>
-      <c r="AE259" s="42" t="s">
-        <v>2712</v>
       </c>
       <c r="AF259" s="5"/>
       <c r="AG259" s="5"/>

</xml_diff>